<commit_message>
update core_sim for collision checking
</commit_message>
<xml_diff>
--- a/miscellaneous/mesh_grid_debugging.xlsx
+++ b/miscellaneous/mesh_grid_debugging.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Desktop\kao_ban_zi\miscellaneous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAD1A407-32FD-4653-981B-5431AD441C4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A061923-136D-4C47-9D35-53049099B7CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0277F893-7310-4137-8DFE-4092AA8D5F45}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1 (5)" sheetId="5" r:id="rId1"/>
-    <sheet name="Sheet1 (4)" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="collision_check" sheetId="6" r:id="rId1"/>
+    <sheet name="first_sim_4" sheetId="5" r:id="rId2"/>
+    <sheet name="first_sim_3" sheetId="4" r:id="rId3"/>
+    <sheet name="first_sim_2" sheetId="3" r:id="rId4"/>
+    <sheet name="first_sim_1" sheetId="2" r:id="rId5"/>
+    <sheet name="first_sim_0" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="1">
   <si>
     <t>Mesh Grid for Game Developing</t>
   </si>
@@ -44,7 +45,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +55,12 @@
     </font>
     <font>
       <sz val="22"/>
+      <color theme="1"/>
+      <name val="Gill Sans MT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Gill Sans MT"/>
       <family val="2"/>
@@ -232,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -262,9 +269,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -298,6 +302,57 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -613,10 +668,2710 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DDE3C2-4051-4279-A224-88B5156F213F}">
+  <dimension ref="A1:BM47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="Q20" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="BP32" sqref="BP32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="32" width="7.140625" style="26"/>
+    <col min="33" max="33" width="7.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="35" max="65" width="7.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="66" max="16384" width="7.140625" style="26"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="25"/>
+    </row>
+    <row r="2" spans="1:32" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28"/>
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="29"/>
+    </row>
+    <row r="3" spans="1:32" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="28"/>
+      <c r="AE3" s="28"/>
+      <c r="AF3" s="29"/>
+    </row>
+    <row r="21" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR21" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="30"/>
+      <c r="AT21" s="30"/>
+      <c r="AU21" s="30"/>
+      <c r="AV21" s="30"/>
+      <c r="AW21" s="30"/>
+      <c r="AX21" s="30"/>
+      <c r="AY21" s="30"/>
+      <c r="AZ21" s="30"/>
+      <c r="BA21" s="30"/>
+      <c r="BB21" s="30"/>
+      <c r="BC21" s="30"/>
+    </row>
+    <row r="22" spans="33:65" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH22" s="26">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="26">
+        <v>1</v>
+      </c>
+      <c r="AJ22" s="26">
+        <v>2</v>
+      </c>
+      <c r="AK22" s="26">
+        <v>3</v>
+      </c>
+      <c r="AL22" s="26">
+        <v>4</v>
+      </c>
+      <c r="AM22" s="26">
+        <v>5</v>
+      </c>
+      <c r="AN22" s="26">
+        <v>6</v>
+      </c>
+      <c r="AO22" s="26">
+        <v>7</v>
+      </c>
+      <c r="AP22" s="26">
+        <v>8</v>
+      </c>
+      <c r="AQ22" s="26">
+        <v>9</v>
+      </c>
+      <c r="AR22" s="26">
+        <v>10</v>
+      </c>
+      <c r="AS22" s="26">
+        <v>11</v>
+      </c>
+      <c r="AT22" s="26">
+        <v>12</v>
+      </c>
+      <c r="AU22" s="26">
+        <v>13</v>
+      </c>
+      <c r="AV22" s="26">
+        <v>14</v>
+      </c>
+      <c r="AW22" s="26">
+        <v>15</v>
+      </c>
+      <c r="AX22" s="26">
+        <v>16</v>
+      </c>
+      <c r="AY22" s="26">
+        <v>17</v>
+      </c>
+      <c r="AZ22" s="26">
+        <v>18</v>
+      </c>
+      <c r="BA22" s="26">
+        <v>19</v>
+      </c>
+      <c r="BB22" s="26">
+        <v>20</v>
+      </c>
+      <c r="BC22" s="26">
+        <v>21</v>
+      </c>
+      <c r="BD22" s="26">
+        <v>22</v>
+      </c>
+      <c r="BE22" s="26">
+        <v>23</v>
+      </c>
+      <c r="BF22" s="26">
+        <v>24</v>
+      </c>
+      <c r="BG22" s="26">
+        <v>25</v>
+      </c>
+      <c r="BH22" s="26">
+        <v>26</v>
+      </c>
+      <c r="BI22" s="26">
+        <v>27</v>
+      </c>
+      <c r="BJ22" s="26">
+        <v>28</v>
+      </c>
+      <c r="BK22" s="26">
+        <v>29</v>
+      </c>
+      <c r="BL22" s="26">
+        <v>30</v>
+      </c>
+      <c r="BM22" s="26">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG23" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="23">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="31">
+        <v>1</v>
+      </c>
+      <c r="AJ23" s="32">
+        <v>2</v>
+      </c>
+      <c r="AK23" s="24">
+        <v>3</v>
+      </c>
+      <c r="AL23" s="24">
+        <v>4</v>
+      </c>
+      <c r="AM23" s="24">
+        <v>5</v>
+      </c>
+      <c r="AN23" s="24">
+        <v>6</v>
+      </c>
+      <c r="AO23" s="24">
+        <v>7</v>
+      </c>
+      <c r="AP23" s="24">
+        <v>8</v>
+      </c>
+      <c r="AQ23" s="24">
+        <v>9</v>
+      </c>
+      <c r="AR23" s="24">
+        <v>10</v>
+      </c>
+      <c r="AS23" s="24">
+        <v>11</v>
+      </c>
+      <c r="AT23" s="24">
+        <v>12</v>
+      </c>
+      <c r="AU23" s="24">
+        <v>13</v>
+      </c>
+      <c r="AV23" s="24">
+        <v>14</v>
+      </c>
+      <c r="AW23" s="24">
+        <v>15</v>
+      </c>
+      <c r="AX23" s="24">
+        <v>16</v>
+      </c>
+      <c r="AY23" s="24">
+        <v>17</v>
+      </c>
+      <c r="AZ23" s="24">
+        <v>18</v>
+      </c>
+      <c r="BA23" s="24">
+        <v>19</v>
+      </c>
+      <c r="BB23" s="24">
+        <v>20</v>
+      </c>
+      <c r="BC23" s="24">
+        <v>21</v>
+      </c>
+      <c r="BD23" s="24">
+        <v>22</v>
+      </c>
+      <c r="BE23" s="24">
+        <v>23</v>
+      </c>
+      <c r="BF23" s="24">
+        <v>24</v>
+      </c>
+      <c r="BG23" s="24">
+        <v>25</v>
+      </c>
+      <c r="BH23" s="24">
+        <v>26</v>
+      </c>
+      <c r="BI23" s="24">
+        <v>27</v>
+      </c>
+      <c r="BJ23" s="24">
+        <v>28</v>
+      </c>
+      <c r="BK23" s="24">
+        <v>29</v>
+      </c>
+      <c r="BL23" s="24">
+        <v>30</v>
+      </c>
+      <c r="BM23" s="25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG24" s="26">
+        <v>1</v>
+      </c>
+      <c r="AH24" s="27">
+        <v>32</v>
+      </c>
+      <c r="AI24" s="28">
+        <v>33</v>
+      </c>
+      <c r="AJ24" s="28">
+        <v>34</v>
+      </c>
+      <c r="AK24" s="33">
+        <v>35</v>
+      </c>
+      <c r="AL24" s="34">
+        <v>36</v>
+      </c>
+      <c r="AM24" s="28">
+        <v>37</v>
+      </c>
+      <c r="AN24" s="28">
+        <v>38</v>
+      </c>
+      <c r="AO24" s="28">
+        <v>39</v>
+      </c>
+      <c r="AP24" s="28">
+        <v>40</v>
+      </c>
+      <c r="AQ24" s="28">
+        <v>41</v>
+      </c>
+      <c r="AR24" s="28">
+        <v>42</v>
+      </c>
+      <c r="AS24" s="28">
+        <v>43</v>
+      </c>
+      <c r="AT24" s="28">
+        <v>44</v>
+      </c>
+      <c r="AU24" s="28">
+        <v>45</v>
+      </c>
+      <c r="AV24" s="28">
+        <v>46</v>
+      </c>
+      <c r="AW24" s="28">
+        <v>47</v>
+      </c>
+      <c r="AX24" s="28">
+        <v>48</v>
+      </c>
+      <c r="AY24" s="28">
+        <v>49</v>
+      </c>
+      <c r="AZ24" s="28">
+        <v>50</v>
+      </c>
+      <c r="BA24" s="28">
+        <v>51</v>
+      </c>
+      <c r="BB24" s="28">
+        <v>52</v>
+      </c>
+      <c r="BC24" s="28">
+        <v>53</v>
+      </c>
+      <c r="BD24" s="28">
+        <v>54</v>
+      </c>
+      <c r="BE24" s="28">
+        <v>55</v>
+      </c>
+      <c r="BF24" s="28">
+        <v>56</v>
+      </c>
+      <c r="BG24" s="28">
+        <v>57</v>
+      </c>
+      <c r="BH24" s="28">
+        <v>58</v>
+      </c>
+      <c r="BI24" s="28">
+        <v>59</v>
+      </c>
+      <c r="BJ24" s="28">
+        <v>60</v>
+      </c>
+      <c r="BK24" s="28">
+        <v>61</v>
+      </c>
+      <c r="BL24" s="28">
+        <v>62</v>
+      </c>
+      <c r="BM24" s="29">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG25" s="26">
+        <v>2</v>
+      </c>
+      <c r="AH25" s="27">
+        <v>64</v>
+      </c>
+      <c r="AI25" s="28">
+        <v>65</v>
+      </c>
+      <c r="AJ25" s="28">
+        <v>66</v>
+      </c>
+      <c r="AK25" s="28">
+        <v>67</v>
+      </c>
+      <c r="AL25" s="28">
+        <v>68</v>
+      </c>
+      <c r="AM25" s="28">
+        <v>69</v>
+      </c>
+      <c r="AN25" s="28">
+        <v>70</v>
+      </c>
+      <c r="AO25" s="28">
+        <v>71</v>
+      </c>
+      <c r="AP25" s="28">
+        <v>72</v>
+      </c>
+      <c r="AQ25" s="28">
+        <v>73</v>
+      </c>
+      <c r="AR25" s="28">
+        <v>74</v>
+      </c>
+      <c r="AS25" s="28">
+        <v>75</v>
+      </c>
+      <c r="AT25" s="28">
+        <v>76</v>
+      </c>
+      <c r="AU25" s="28">
+        <v>77</v>
+      </c>
+      <c r="AV25" s="28">
+        <v>78</v>
+      </c>
+      <c r="AW25" s="28">
+        <v>79</v>
+      </c>
+      <c r="AX25" s="28">
+        <v>80</v>
+      </c>
+      <c r="AY25" s="28">
+        <v>81</v>
+      </c>
+      <c r="AZ25" s="28">
+        <v>82</v>
+      </c>
+      <c r="BA25" s="28">
+        <v>83</v>
+      </c>
+      <c r="BB25" s="28">
+        <v>84</v>
+      </c>
+      <c r="BC25" s="28">
+        <v>85</v>
+      </c>
+      <c r="BD25" s="28">
+        <v>86</v>
+      </c>
+      <c r="BE25" s="28">
+        <v>87</v>
+      </c>
+      <c r="BF25" s="28">
+        <v>88</v>
+      </c>
+      <c r="BG25" s="28">
+        <v>89</v>
+      </c>
+      <c r="BH25" s="28">
+        <v>90</v>
+      </c>
+      <c r="BI25" s="28">
+        <v>91</v>
+      </c>
+      <c r="BJ25" s="28">
+        <v>92</v>
+      </c>
+      <c r="BK25" s="28">
+        <v>93</v>
+      </c>
+      <c r="BL25" s="28">
+        <v>94</v>
+      </c>
+      <c r="BM25" s="29">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG26" s="26">
+        <v>3</v>
+      </c>
+      <c r="AH26" s="27">
+        <v>96</v>
+      </c>
+      <c r="AI26" s="28">
+        <v>97</v>
+      </c>
+      <c r="AJ26" s="28">
+        <v>98</v>
+      </c>
+      <c r="AK26" s="28">
+        <v>99</v>
+      </c>
+      <c r="AL26" s="28">
+        <v>100</v>
+      </c>
+      <c r="AM26" s="28">
+        <v>101</v>
+      </c>
+      <c r="AN26" s="28">
+        <v>102</v>
+      </c>
+      <c r="AO26" s="28">
+        <v>103</v>
+      </c>
+      <c r="AP26" s="28">
+        <v>104</v>
+      </c>
+      <c r="AQ26" s="28">
+        <v>105</v>
+      </c>
+      <c r="AR26" s="28">
+        <v>106</v>
+      </c>
+      <c r="AS26" s="28">
+        <v>107</v>
+      </c>
+      <c r="AT26" s="28">
+        <v>108</v>
+      </c>
+      <c r="AU26" s="28">
+        <v>109</v>
+      </c>
+      <c r="AV26" s="28">
+        <v>110</v>
+      </c>
+      <c r="AW26" s="28">
+        <v>111</v>
+      </c>
+      <c r="AX26" s="28">
+        <v>112</v>
+      </c>
+      <c r="AY26" s="28">
+        <v>113</v>
+      </c>
+      <c r="AZ26" s="28">
+        <v>114</v>
+      </c>
+      <c r="BA26" s="28">
+        <v>115</v>
+      </c>
+      <c r="BB26" s="28">
+        <v>116</v>
+      </c>
+      <c r="BC26" s="28">
+        <v>117</v>
+      </c>
+      <c r="BD26" s="28">
+        <v>118</v>
+      </c>
+      <c r="BE26" s="28">
+        <v>119</v>
+      </c>
+      <c r="BF26" s="28">
+        <v>120</v>
+      </c>
+      <c r="BG26" s="28">
+        <v>121</v>
+      </c>
+      <c r="BH26" s="28">
+        <v>122</v>
+      </c>
+      <c r="BI26" s="28">
+        <v>123</v>
+      </c>
+      <c r="BJ26" s="28">
+        <v>124</v>
+      </c>
+      <c r="BK26" s="28">
+        <v>125</v>
+      </c>
+      <c r="BL26" s="28">
+        <v>126</v>
+      </c>
+      <c r="BM26" s="29">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG27" s="26">
+        <v>4</v>
+      </c>
+      <c r="AH27" s="27">
+        <v>128</v>
+      </c>
+      <c r="AI27" s="28">
+        <v>129</v>
+      </c>
+      <c r="AJ27" s="28">
+        <v>130</v>
+      </c>
+      <c r="AK27" s="28">
+        <v>131</v>
+      </c>
+      <c r="AL27" s="28">
+        <v>132</v>
+      </c>
+      <c r="AM27" s="28">
+        <v>133</v>
+      </c>
+      <c r="AN27" s="28">
+        <v>134</v>
+      </c>
+      <c r="AO27" s="28">
+        <v>135</v>
+      </c>
+      <c r="AP27" s="28">
+        <v>136</v>
+      </c>
+      <c r="AQ27" s="28">
+        <v>137</v>
+      </c>
+      <c r="AR27" s="28">
+        <v>138</v>
+      </c>
+      <c r="AS27" s="28">
+        <v>139</v>
+      </c>
+      <c r="AT27" s="28">
+        <v>140</v>
+      </c>
+      <c r="AU27" s="28">
+        <v>141</v>
+      </c>
+      <c r="AV27" s="28">
+        <v>142</v>
+      </c>
+      <c r="AW27" s="28">
+        <v>143</v>
+      </c>
+      <c r="AX27" s="28">
+        <v>144</v>
+      </c>
+      <c r="AY27" s="28">
+        <v>145</v>
+      </c>
+      <c r="AZ27" s="28">
+        <v>146</v>
+      </c>
+      <c r="BA27" s="28">
+        <v>147</v>
+      </c>
+      <c r="BB27" s="28">
+        <v>148</v>
+      </c>
+      <c r="BC27" s="28">
+        <v>149</v>
+      </c>
+      <c r="BD27" s="28">
+        <v>150</v>
+      </c>
+      <c r="BE27" s="28">
+        <v>151</v>
+      </c>
+      <c r="BF27" s="28">
+        <v>152</v>
+      </c>
+      <c r="BG27" s="28">
+        <v>153</v>
+      </c>
+      <c r="BH27" s="28">
+        <v>154</v>
+      </c>
+      <c r="BI27" s="28">
+        <v>155</v>
+      </c>
+      <c r="BJ27" s="28">
+        <v>156</v>
+      </c>
+      <c r="BK27" s="28">
+        <v>157</v>
+      </c>
+      <c r="BL27" s="28">
+        <v>158</v>
+      </c>
+      <c r="BM27" s="29">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG28" s="26">
+        <v>5</v>
+      </c>
+      <c r="AH28" s="27">
+        <v>160</v>
+      </c>
+      <c r="AI28" s="28">
+        <v>161</v>
+      </c>
+      <c r="AJ28" s="28">
+        <v>162</v>
+      </c>
+      <c r="AK28" s="28">
+        <v>163</v>
+      </c>
+      <c r="AL28" s="28">
+        <v>164</v>
+      </c>
+      <c r="AM28" s="28">
+        <v>165</v>
+      </c>
+      <c r="AN28" s="28">
+        <v>166</v>
+      </c>
+      <c r="AO28" s="28">
+        <v>167</v>
+      </c>
+      <c r="AP28" s="28">
+        <v>168</v>
+      </c>
+      <c r="AQ28" s="28">
+        <v>169</v>
+      </c>
+      <c r="AR28" s="28">
+        <v>170</v>
+      </c>
+      <c r="AS28" s="28">
+        <v>171</v>
+      </c>
+      <c r="AT28" s="28">
+        <v>172</v>
+      </c>
+      <c r="AU28" s="28">
+        <v>173</v>
+      </c>
+      <c r="AV28" s="28">
+        <v>174</v>
+      </c>
+      <c r="AW28" s="28">
+        <v>175</v>
+      </c>
+      <c r="AX28" s="28">
+        <v>176</v>
+      </c>
+      <c r="AY28" s="28">
+        <v>177</v>
+      </c>
+      <c r="AZ28" s="28">
+        <v>178</v>
+      </c>
+      <c r="BA28" s="28">
+        <v>179</v>
+      </c>
+      <c r="BB28" s="28">
+        <v>180</v>
+      </c>
+      <c r="BC28" s="28">
+        <v>181</v>
+      </c>
+      <c r="BD28" s="28">
+        <v>182</v>
+      </c>
+      <c r="BE28" s="28">
+        <v>183</v>
+      </c>
+      <c r="BF28" s="28">
+        <v>184</v>
+      </c>
+      <c r="BG28" s="28">
+        <v>185</v>
+      </c>
+      <c r="BH28" s="28">
+        <v>186</v>
+      </c>
+      <c r="BI28" s="28">
+        <v>187</v>
+      </c>
+      <c r="BJ28" s="28">
+        <v>188</v>
+      </c>
+      <c r="BK28" s="28">
+        <v>189</v>
+      </c>
+      <c r="BL28" s="28">
+        <v>190</v>
+      </c>
+      <c r="BM28" s="29">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG29" s="26">
+        <v>6</v>
+      </c>
+      <c r="AH29" s="27">
+        <v>192</v>
+      </c>
+      <c r="AI29" s="28">
+        <v>193</v>
+      </c>
+      <c r="AJ29" s="28">
+        <v>194</v>
+      </c>
+      <c r="AK29" s="28">
+        <v>195</v>
+      </c>
+      <c r="AL29" s="28">
+        <v>196</v>
+      </c>
+      <c r="AM29" s="28">
+        <v>197</v>
+      </c>
+      <c r="AN29" s="28">
+        <v>198</v>
+      </c>
+      <c r="AO29" s="28">
+        <v>199</v>
+      </c>
+      <c r="AP29" s="28">
+        <v>200</v>
+      </c>
+      <c r="AQ29" s="28">
+        <v>201</v>
+      </c>
+      <c r="AR29" s="28">
+        <v>202</v>
+      </c>
+      <c r="AS29" s="28">
+        <v>203</v>
+      </c>
+      <c r="AT29" s="28">
+        <v>204</v>
+      </c>
+      <c r="AU29" s="28">
+        <v>205</v>
+      </c>
+      <c r="AV29" s="28">
+        <v>206</v>
+      </c>
+      <c r="AW29" s="28">
+        <v>207</v>
+      </c>
+      <c r="AX29" s="28">
+        <v>208</v>
+      </c>
+      <c r="AY29" s="28">
+        <v>209</v>
+      </c>
+      <c r="AZ29" s="28">
+        <v>210</v>
+      </c>
+      <c r="BA29" s="28">
+        <v>211</v>
+      </c>
+      <c r="BB29" s="28">
+        <v>212</v>
+      </c>
+      <c r="BC29" s="28">
+        <v>213</v>
+      </c>
+      <c r="BD29" s="28">
+        <v>214</v>
+      </c>
+      <c r="BE29" s="28">
+        <v>215</v>
+      </c>
+      <c r="BF29" s="28">
+        <v>216</v>
+      </c>
+      <c r="BG29" s="28">
+        <v>217</v>
+      </c>
+      <c r="BH29" s="28">
+        <v>218</v>
+      </c>
+      <c r="BI29" s="28">
+        <v>219</v>
+      </c>
+      <c r="BJ29" s="28">
+        <v>220</v>
+      </c>
+      <c r="BK29" s="28">
+        <v>221</v>
+      </c>
+      <c r="BL29" s="28">
+        <v>222</v>
+      </c>
+      <c r="BM29" s="29">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG30" s="26">
+        <v>7</v>
+      </c>
+      <c r="AH30" s="27">
+        <v>224</v>
+      </c>
+      <c r="AI30" s="28">
+        <v>225</v>
+      </c>
+      <c r="AJ30" s="28">
+        <v>226</v>
+      </c>
+      <c r="AK30" s="28">
+        <v>227</v>
+      </c>
+      <c r="AL30" s="28">
+        <v>228</v>
+      </c>
+      <c r="AM30" s="28">
+        <v>229</v>
+      </c>
+      <c r="AN30" s="28">
+        <v>230</v>
+      </c>
+      <c r="AO30" s="28">
+        <v>231</v>
+      </c>
+      <c r="AP30" s="28">
+        <v>232</v>
+      </c>
+      <c r="AQ30" s="28">
+        <v>233</v>
+      </c>
+      <c r="AR30" s="28">
+        <v>234</v>
+      </c>
+      <c r="AS30" s="28">
+        <v>235</v>
+      </c>
+      <c r="AT30" s="28">
+        <v>236</v>
+      </c>
+      <c r="AU30" s="28">
+        <v>237</v>
+      </c>
+      <c r="AV30" s="28">
+        <v>238</v>
+      </c>
+      <c r="AW30" s="28">
+        <v>239</v>
+      </c>
+      <c r="AX30" s="28">
+        <v>240</v>
+      </c>
+      <c r="AY30" s="28">
+        <v>241</v>
+      </c>
+      <c r="AZ30" s="28">
+        <v>242</v>
+      </c>
+      <c r="BA30" s="28">
+        <v>243</v>
+      </c>
+      <c r="BB30" s="28">
+        <v>244</v>
+      </c>
+      <c r="BC30" s="28">
+        <v>245</v>
+      </c>
+      <c r="BD30" s="28">
+        <v>246</v>
+      </c>
+      <c r="BE30" s="28">
+        <v>247</v>
+      </c>
+      <c r="BF30" s="28">
+        <v>248</v>
+      </c>
+      <c r="BG30" s="28">
+        <v>249</v>
+      </c>
+      <c r="BH30" s="28">
+        <v>250</v>
+      </c>
+      <c r="BI30" s="28">
+        <v>251</v>
+      </c>
+      <c r="BJ30" s="28">
+        <v>252</v>
+      </c>
+      <c r="BK30" s="28">
+        <v>253</v>
+      </c>
+      <c r="BL30" s="28">
+        <v>254</v>
+      </c>
+      <c r="BM30" s="29">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG31" s="26">
+        <v>8</v>
+      </c>
+      <c r="AH31" s="27">
+        <v>256</v>
+      </c>
+      <c r="AI31" s="28">
+        <v>257</v>
+      </c>
+      <c r="AJ31" s="28">
+        <v>258</v>
+      </c>
+      <c r="AK31" s="28">
+        <v>259</v>
+      </c>
+      <c r="AL31" s="28">
+        <v>260</v>
+      </c>
+      <c r="AM31" s="28">
+        <v>261</v>
+      </c>
+      <c r="AN31" s="28">
+        <v>262</v>
+      </c>
+      <c r="AO31" s="28">
+        <v>263</v>
+      </c>
+      <c r="AP31" s="28">
+        <v>264</v>
+      </c>
+      <c r="AQ31" s="28">
+        <v>265</v>
+      </c>
+      <c r="AR31" s="28">
+        <v>266</v>
+      </c>
+      <c r="AS31" s="28">
+        <v>267</v>
+      </c>
+      <c r="AT31" s="28">
+        <v>268</v>
+      </c>
+      <c r="AU31" s="28">
+        <v>269</v>
+      </c>
+      <c r="AV31" s="28">
+        <v>270</v>
+      </c>
+      <c r="AW31" s="28">
+        <v>271</v>
+      </c>
+      <c r="AX31" s="28">
+        <v>272</v>
+      </c>
+      <c r="AY31" s="28">
+        <v>273</v>
+      </c>
+      <c r="AZ31" s="28">
+        <v>274</v>
+      </c>
+      <c r="BA31" s="28">
+        <v>275</v>
+      </c>
+      <c r="BB31" s="28">
+        <v>276</v>
+      </c>
+      <c r="BC31" s="28">
+        <v>277</v>
+      </c>
+      <c r="BD31" s="28">
+        <v>278</v>
+      </c>
+      <c r="BE31" s="28">
+        <v>279</v>
+      </c>
+      <c r="BF31" s="28">
+        <v>280</v>
+      </c>
+      <c r="BG31" s="28">
+        <v>281</v>
+      </c>
+      <c r="BH31" s="28">
+        <v>282</v>
+      </c>
+      <c r="BI31" s="28">
+        <v>283</v>
+      </c>
+      <c r="BJ31" s="28">
+        <v>284</v>
+      </c>
+      <c r="BK31" s="28">
+        <v>285</v>
+      </c>
+      <c r="BL31" s="28">
+        <v>286</v>
+      </c>
+      <c r="BM31" s="29">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="32" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG32" s="26">
+        <v>9</v>
+      </c>
+      <c r="AH32" s="27">
+        <v>288</v>
+      </c>
+      <c r="AI32" s="28">
+        <v>289</v>
+      </c>
+      <c r="AJ32" s="28">
+        <v>290</v>
+      </c>
+      <c r="AK32" s="28">
+        <v>291</v>
+      </c>
+      <c r="AL32" s="28">
+        <v>292</v>
+      </c>
+      <c r="AM32" s="28">
+        <v>293</v>
+      </c>
+      <c r="AN32" s="28">
+        <v>294</v>
+      </c>
+      <c r="AO32" s="28">
+        <v>295</v>
+      </c>
+      <c r="AP32" s="28">
+        <v>296</v>
+      </c>
+      <c r="AQ32" s="28">
+        <v>297</v>
+      </c>
+      <c r="AR32" s="28">
+        <v>298</v>
+      </c>
+      <c r="AS32" s="28">
+        <v>299</v>
+      </c>
+      <c r="AT32" s="28">
+        <v>300</v>
+      </c>
+      <c r="AU32" s="28">
+        <v>301</v>
+      </c>
+      <c r="AV32" s="28">
+        <v>302</v>
+      </c>
+      <c r="AW32" s="28">
+        <v>303</v>
+      </c>
+      <c r="AX32" s="28">
+        <v>304</v>
+      </c>
+      <c r="AY32" s="28">
+        <v>305</v>
+      </c>
+      <c r="AZ32" s="28">
+        <v>306</v>
+      </c>
+      <c r="BA32" s="28">
+        <v>307</v>
+      </c>
+      <c r="BB32" s="28">
+        <v>308</v>
+      </c>
+      <c r="BC32" s="28">
+        <v>309</v>
+      </c>
+      <c r="BD32" s="28">
+        <v>310</v>
+      </c>
+      <c r="BE32" s="28">
+        <v>311</v>
+      </c>
+      <c r="BF32" s="28">
+        <v>312</v>
+      </c>
+      <c r="BG32" s="28">
+        <v>313</v>
+      </c>
+      <c r="BH32" s="28">
+        <v>314</v>
+      </c>
+      <c r="BI32" s="28">
+        <v>315</v>
+      </c>
+      <c r="BJ32" s="28">
+        <v>316</v>
+      </c>
+      <c r="BK32" s="28">
+        <v>317</v>
+      </c>
+      <c r="BL32" s="28">
+        <v>318</v>
+      </c>
+      <c r="BM32" s="29">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="33" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG33" s="26">
+        <v>10</v>
+      </c>
+      <c r="AH33" s="27">
+        <v>320</v>
+      </c>
+      <c r="AI33" s="28">
+        <v>321</v>
+      </c>
+      <c r="AJ33" s="28">
+        <v>322</v>
+      </c>
+      <c r="AK33" s="28">
+        <v>323</v>
+      </c>
+      <c r="AL33" s="28">
+        <v>324</v>
+      </c>
+      <c r="AM33" s="28">
+        <v>325</v>
+      </c>
+      <c r="AN33" s="28">
+        <v>326</v>
+      </c>
+      <c r="AO33" s="28">
+        <v>327</v>
+      </c>
+      <c r="AP33" s="28">
+        <v>328</v>
+      </c>
+      <c r="AQ33" s="28">
+        <v>329</v>
+      </c>
+      <c r="AR33" s="28">
+        <v>330</v>
+      </c>
+      <c r="AS33" s="28">
+        <v>331</v>
+      </c>
+      <c r="AT33" s="28">
+        <v>332</v>
+      </c>
+      <c r="AU33" s="28">
+        <v>333</v>
+      </c>
+      <c r="AV33" s="28">
+        <v>334</v>
+      </c>
+      <c r="AW33" s="28">
+        <v>335</v>
+      </c>
+      <c r="AX33" s="28">
+        <v>336</v>
+      </c>
+      <c r="AY33" s="28">
+        <v>337</v>
+      </c>
+      <c r="AZ33" s="28">
+        <v>338</v>
+      </c>
+      <c r="BA33" s="28">
+        <v>339</v>
+      </c>
+      <c r="BB33" s="28">
+        <v>340</v>
+      </c>
+      <c r="BC33" s="28">
+        <v>341</v>
+      </c>
+      <c r="BD33" s="28">
+        <v>342</v>
+      </c>
+      <c r="BE33" s="28">
+        <v>343</v>
+      </c>
+      <c r="BF33" s="28">
+        <v>344</v>
+      </c>
+      <c r="BG33" s="28">
+        <v>345</v>
+      </c>
+      <c r="BH33" s="28">
+        <v>346</v>
+      </c>
+      <c r="BI33" s="28">
+        <v>347</v>
+      </c>
+      <c r="BJ33" s="28">
+        <v>348</v>
+      </c>
+      <c r="BK33" s="28">
+        <v>349</v>
+      </c>
+      <c r="BL33" s="28">
+        <v>350</v>
+      </c>
+      <c r="BM33" s="29">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="34" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG34" s="26">
+        <v>11</v>
+      </c>
+      <c r="AH34" s="27">
+        <v>352</v>
+      </c>
+      <c r="AI34" s="28">
+        <v>353</v>
+      </c>
+      <c r="AJ34" s="28">
+        <v>354</v>
+      </c>
+      <c r="AK34" s="28">
+        <v>355</v>
+      </c>
+      <c r="AL34" s="28">
+        <v>356</v>
+      </c>
+      <c r="AM34" s="28">
+        <v>357</v>
+      </c>
+      <c r="AN34" s="28">
+        <v>358</v>
+      </c>
+      <c r="AO34" s="28">
+        <v>359</v>
+      </c>
+      <c r="AP34" s="28">
+        <v>360</v>
+      </c>
+      <c r="AQ34" s="28">
+        <v>361</v>
+      </c>
+      <c r="AR34" s="28">
+        <v>362</v>
+      </c>
+      <c r="AS34" s="28">
+        <v>363</v>
+      </c>
+      <c r="AT34" s="28">
+        <v>364</v>
+      </c>
+      <c r="AU34" s="28">
+        <v>365</v>
+      </c>
+      <c r="AV34" s="28">
+        <v>366</v>
+      </c>
+      <c r="AW34" s="28">
+        <v>367</v>
+      </c>
+      <c r="AX34" s="28">
+        <v>368</v>
+      </c>
+      <c r="AY34" s="28">
+        <v>369</v>
+      </c>
+      <c r="AZ34" s="28">
+        <v>370</v>
+      </c>
+      <c r="BA34" s="28">
+        <v>371</v>
+      </c>
+      <c r="BB34" s="28">
+        <v>372</v>
+      </c>
+      <c r="BC34" s="28">
+        <v>373</v>
+      </c>
+      <c r="BD34" s="28">
+        <v>374</v>
+      </c>
+      <c r="BE34" s="28">
+        <v>375</v>
+      </c>
+      <c r="BF34" s="28">
+        <v>376</v>
+      </c>
+      <c r="BG34" s="28">
+        <v>377</v>
+      </c>
+      <c r="BH34" s="28">
+        <v>378</v>
+      </c>
+      <c r="BI34" s="28">
+        <v>379</v>
+      </c>
+      <c r="BJ34" s="28">
+        <v>380</v>
+      </c>
+      <c r="BK34" s="28">
+        <v>381</v>
+      </c>
+      <c r="BL34" s="28">
+        <v>382</v>
+      </c>
+      <c r="BM34" s="29">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="35" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG35" s="26">
+        <v>12</v>
+      </c>
+      <c r="AH35" s="27">
+        <v>384</v>
+      </c>
+      <c r="AI35" s="28">
+        <v>385</v>
+      </c>
+      <c r="AJ35" s="28">
+        <v>386</v>
+      </c>
+      <c r="AK35" s="28">
+        <v>387</v>
+      </c>
+      <c r="AL35" s="28">
+        <v>388</v>
+      </c>
+      <c r="AM35" s="28">
+        <v>389</v>
+      </c>
+      <c r="AN35" s="28">
+        <v>390</v>
+      </c>
+      <c r="AO35" s="28">
+        <v>391</v>
+      </c>
+      <c r="AP35" s="28">
+        <v>392</v>
+      </c>
+      <c r="AQ35" s="28">
+        <v>393</v>
+      </c>
+      <c r="AR35" s="28">
+        <v>394</v>
+      </c>
+      <c r="AS35" s="28">
+        <v>395</v>
+      </c>
+      <c r="AT35" s="28">
+        <v>396</v>
+      </c>
+      <c r="AU35" s="28">
+        <v>397</v>
+      </c>
+      <c r="AV35" s="28">
+        <v>398</v>
+      </c>
+      <c r="AW35" s="28">
+        <v>399</v>
+      </c>
+      <c r="AX35" s="28">
+        <v>400</v>
+      </c>
+      <c r="AY35" s="28">
+        <v>401</v>
+      </c>
+      <c r="AZ35" s="28">
+        <v>402</v>
+      </c>
+      <c r="BA35" s="28">
+        <v>403</v>
+      </c>
+      <c r="BB35" s="28">
+        <v>404</v>
+      </c>
+      <c r="BC35" s="28">
+        <v>405</v>
+      </c>
+      <c r="BD35" s="28">
+        <v>406</v>
+      </c>
+      <c r="BE35" s="28">
+        <v>407</v>
+      </c>
+      <c r="BF35" s="28">
+        <v>408</v>
+      </c>
+      <c r="BG35" s="28">
+        <v>409</v>
+      </c>
+      <c r="BH35" s="28">
+        <v>410</v>
+      </c>
+      <c r="BI35" s="28">
+        <v>411</v>
+      </c>
+      <c r="BJ35" s="28">
+        <v>412</v>
+      </c>
+      <c r="BK35" s="28">
+        <v>413</v>
+      </c>
+      <c r="BL35" s="28">
+        <v>414</v>
+      </c>
+      <c r="BM35" s="29">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="36" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG36" s="26">
+        <v>13</v>
+      </c>
+      <c r="AH36" s="27">
+        <v>416</v>
+      </c>
+      <c r="AI36" s="28">
+        <v>417</v>
+      </c>
+      <c r="AJ36" s="28">
+        <v>418</v>
+      </c>
+      <c r="AK36" s="28">
+        <v>419</v>
+      </c>
+      <c r="AL36" s="28">
+        <v>420</v>
+      </c>
+      <c r="AM36" s="28">
+        <v>421</v>
+      </c>
+      <c r="AN36" s="28">
+        <v>422</v>
+      </c>
+      <c r="AO36" s="28">
+        <v>423</v>
+      </c>
+      <c r="AP36" s="28">
+        <v>424</v>
+      </c>
+      <c r="AQ36" s="28">
+        <v>425</v>
+      </c>
+      <c r="AR36" s="28">
+        <v>426</v>
+      </c>
+      <c r="AS36" s="28">
+        <v>427</v>
+      </c>
+      <c r="AT36" s="28">
+        <v>428</v>
+      </c>
+      <c r="AU36" s="28">
+        <v>429</v>
+      </c>
+      <c r="AV36" s="28">
+        <v>430</v>
+      </c>
+      <c r="AW36" s="28">
+        <v>431</v>
+      </c>
+      <c r="AX36" s="28">
+        <v>432</v>
+      </c>
+      <c r="AY36" s="28">
+        <v>433</v>
+      </c>
+      <c r="AZ36" s="28">
+        <v>434</v>
+      </c>
+      <c r="BA36" s="28">
+        <v>435</v>
+      </c>
+      <c r="BB36" s="28">
+        <v>436</v>
+      </c>
+      <c r="BC36" s="28">
+        <v>437</v>
+      </c>
+      <c r="BD36" s="28">
+        <v>438</v>
+      </c>
+      <c r="BE36" s="28">
+        <v>439</v>
+      </c>
+      <c r="BF36" s="28">
+        <v>440</v>
+      </c>
+      <c r="BG36" s="28">
+        <v>441</v>
+      </c>
+      <c r="BH36" s="28">
+        <v>442</v>
+      </c>
+      <c r="BI36" s="28">
+        <v>443</v>
+      </c>
+      <c r="BJ36" s="28">
+        <v>444</v>
+      </c>
+      <c r="BK36" s="28">
+        <v>445</v>
+      </c>
+      <c r="BL36" s="28">
+        <v>446</v>
+      </c>
+      <c r="BM36" s="29">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="37" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG37" s="26">
+        <v>14</v>
+      </c>
+      <c r="AH37" s="27">
+        <v>448</v>
+      </c>
+      <c r="AI37" s="28">
+        <v>449</v>
+      </c>
+      <c r="AJ37" s="28">
+        <v>450</v>
+      </c>
+      <c r="AK37" s="28">
+        <v>451</v>
+      </c>
+      <c r="AL37" s="28">
+        <v>452</v>
+      </c>
+      <c r="AM37" s="28">
+        <v>453</v>
+      </c>
+      <c r="AN37" s="28">
+        <v>454</v>
+      </c>
+      <c r="AO37" s="28">
+        <v>455</v>
+      </c>
+      <c r="AP37" s="28">
+        <v>456</v>
+      </c>
+      <c r="AQ37" s="28">
+        <v>457</v>
+      </c>
+      <c r="AR37" s="28">
+        <v>458</v>
+      </c>
+      <c r="AS37" s="28">
+        <v>459</v>
+      </c>
+      <c r="AT37" s="28">
+        <v>460</v>
+      </c>
+      <c r="AU37" s="28">
+        <v>461</v>
+      </c>
+      <c r="AV37" s="28">
+        <v>462</v>
+      </c>
+      <c r="AW37" s="28">
+        <v>463</v>
+      </c>
+      <c r="AX37" s="28">
+        <v>464</v>
+      </c>
+      <c r="AY37" s="28">
+        <v>465</v>
+      </c>
+      <c r="AZ37" s="28">
+        <v>466</v>
+      </c>
+      <c r="BA37" s="28">
+        <v>467</v>
+      </c>
+      <c r="BB37" s="28">
+        <v>468</v>
+      </c>
+      <c r="BC37" s="28">
+        <v>469</v>
+      </c>
+      <c r="BD37" s="28">
+        <v>470</v>
+      </c>
+      <c r="BE37" s="28">
+        <v>471</v>
+      </c>
+      <c r="BF37" s="28">
+        <v>472</v>
+      </c>
+      <c r="BG37" s="28">
+        <v>473</v>
+      </c>
+      <c r="BH37" s="28">
+        <v>474</v>
+      </c>
+      <c r="BI37" s="28">
+        <v>475</v>
+      </c>
+      <c r="BJ37" s="28">
+        <v>476</v>
+      </c>
+      <c r="BK37" s="28">
+        <v>477</v>
+      </c>
+      <c r="BL37" s="28">
+        <v>478</v>
+      </c>
+      <c r="BM37" s="29">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="38" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG38" s="26">
+        <v>15</v>
+      </c>
+      <c r="AH38" s="27">
+        <v>480</v>
+      </c>
+      <c r="AI38" s="28">
+        <v>481</v>
+      </c>
+      <c r="AJ38" s="28">
+        <v>482</v>
+      </c>
+      <c r="AK38" s="28">
+        <v>483</v>
+      </c>
+      <c r="AL38" s="28">
+        <v>484</v>
+      </c>
+      <c r="AM38" s="28">
+        <v>485</v>
+      </c>
+      <c r="AN38" s="28">
+        <v>486</v>
+      </c>
+      <c r="AO38" s="28">
+        <v>487</v>
+      </c>
+      <c r="AP38" s="28">
+        <v>488</v>
+      </c>
+      <c r="AQ38" s="28">
+        <v>489</v>
+      </c>
+      <c r="AR38" s="28">
+        <v>490</v>
+      </c>
+      <c r="AS38" s="28">
+        <v>491</v>
+      </c>
+      <c r="AT38" s="28">
+        <v>492</v>
+      </c>
+      <c r="AU38" s="28">
+        <v>493</v>
+      </c>
+      <c r="AV38" s="28">
+        <v>494</v>
+      </c>
+      <c r="AW38" s="28">
+        <v>495</v>
+      </c>
+      <c r="AX38" s="28">
+        <v>496</v>
+      </c>
+      <c r="AY38" s="28">
+        <v>497</v>
+      </c>
+      <c r="AZ38" s="28">
+        <v>498</v>
+      </c>
+      <c r="BA38" s="28">
+        <v>499</v>
+      </c>
+      <c r="BB38" s="28">
+        <v>500</v>
+      </c>
+      <c r="BC38" s="28">
+        <v>501</v>
+      </c>
+      <c r="BD38" s="28">
+        <v>502</v>
+      </c>
+      <c r="BE38" s="28">
+        <v>503</v>
+      </c>
+      <c r="BF38" s="28">
+        <v>504</v>
+      </c>
+      <c r="BG38" s="28">
+        <v>505</v>
+      </c>
+      <c r="BH38" s="28">
+        <v>506</v>
+      </c>
+      <c r="BI38" s="28">
+        <v>507</v>
+      </c>
+      <c r="BJ38" s="28">
+        <v>508</v>
+      </c>
+      <c r="BK38" s="28">
+        <v>509</v>
+      </c>
+      <c r="BL38" s="28">
+        <v>510</v>
+      </c>
+      <c r="BM38" s="29">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="39" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG39" s="26">
+        <v>16</v>
+      </c>
+      <c r="AH39" s="27">
+        <v>512</v>
+      </c>
+      <c r="AI39" s="28">
+        <v>513</v>
+      </c>
+      <c r="AJ39" s="28">
+        <v>514</v>
+      </c>
+      <c r="AK39" s="28">
+        <v>515</v>
+      </c>
+      <c r="AL39" s="28">
+        <v>516</v>
+      </c>
+      <c r="AM39" s="28">
+        <v>517</v>
+      </c>
+      <c r="AN39" s="28">
+        <v>518</v>
+      </c>
+      <c r="AO39" s="28">
+        <v>519</v>
+      </c>
+      <c r="AP39" s="28">
+        <v>520</v>
+      </c>
+      <c r="AQ39" s="28">
+        <v>521</v>
+      </c>
+      <c r="AR39" s="28">
+        <v>522</v>
+      </c>
+      <c r="AS39" s="28">
+        <v>523</v>
+      </c>
+      <c r="AT39" s="28">
+        <v>524</v>
+      </c>
+      <c r="AU39" s="28">
+        <v>525</v>
+      </c>
+      <c r="AV39" s="28">
+        <v>526</v>
+      </c>
+      <c r="AW39" s="28">
+        <v>527</v>
+      </c>
+      <c r="AX39" s="28">
+        <v>528</v>
+      </c>
+      <c r="AY39" s="28">
+        <v>529</v>
+      </c>
+      <c r="AZ39" s="28">
+        <v>530</v>
+      </c>
+      <c r="BA39" s="28">
+        <v>531</v>
+      </c>
+      <c r="BB39" s="28">
+        <v>532</v>
+      </c>
+      <c r="BC39" s="28">
+        <v>533</v>
+      </c>
+      <c r="BD39" s="28">
+        <v>534</v>
+      </c>
+      <c r="BE39" s="28">
+        <v>535</v>
+      </c>
+      <c r="BF39" s="28">
+        <v>536</v>
+      </c>
+      <c r="BG39" s="28">
+        <v>537</v>
+      </c>
+      <c r="BH39" s="28">
+        <v>538</v>
+      </c>
+      <c r="BI39" s="28">
+        <v>539</v>
+      </c>
+      <c r="BJ39" s="28">
+        <v>540</v>
+      </c>
+      <c r="BK39" s="28">
+        <v>541</v>
+      </c>
+      <c r="BL39" s="28">
+        <v>542</v>
+      </c>
+      <c r="BM39" s="29">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="40" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG40" s="26">
+        <v>17</v>
+      </c>
+      <c r="AH40" s="27">
+        <v>544</v>
+      </c>
+      <c r="AI40" s="28">
+        <v>545</v>
+      </c>
+      <c r="AJ40" s="28">
+        <v>546</v>
+      </c>
+      <c r="AK40" s="28">
+        <v>547</v>
+      </c>
+      <c r="AL40" s="28">
+        <v>548</v>
+      </c>
+      <c r="AM40" s="28">
+        <v>549</v>
+      </c>
+      <c r="AN40" s="28">
+        <v>550</v>
+      </c>
+      <c r="AO40" s="28">
+        <v>551</v>
+      </c>
+      <c r="AP40" s="28">
+        <v>552</v>
+      </c>
+      <c r="AQ40" s="28">
+        <v>553</v>
+      </c>
+      <c r="AR40" s="28">
+        <v>554</v>
+      </c>
+      <c r="AS40" s="28">
+        <v>555</v>
+      </c>
+      <c r="AT40" s="28">
+        <v>556</v>
+      </c>
+      <c r="AU40" s="28">
+        <v>557</v>
+      </c>
+      <c r="AV40" s="28">
+        <v>558</v>
+      </c>
+      <c r="AW40" s="28">
+        <v>559</v>
+      </c>
+      <c r="AX40" s="28">
+        <v>560</v>
+      </c>
+      <c r="AY40" s="28">
+        <v>561</v>
+      </c>
+      <c r="AZ40" s="28">
+        <v>562</v>
+      </c>
+      <c r="BA40" s="28">
+        <v>563</v>
+      </c>
+      <c r="BB40" s="28">
+        <v>564</v>
+      </c>
+      <c r="BC40" s="28">
+        <v>565</v>
+      </c>
+      <c r="BD40" s="28">
+        <v>566</v>
+      </c>
+      <c r="BE40" s="28">
+        <v>567</v>
+      </c>
+      <c r="BF40" s="28">
+        <v>568</v>
+      </c>
+      <c r="BG40" s="28">
+        <v>569</v>
+      </c>
+      <c r="BH40" s="28">
+        <v>570</v>
+      </c>
+      <c r="BI40" s="28">
+        <v>571</v>
+      </c>
+      <c r="BJ40" s="28">
+        <v>572</v>
+      </c>
+      <c r="BK40" s="28">
+        <v>573</v>
+      </c>
+      <c r="BL40" s="28">
+        <v>574</v>
+      </c>
+      <c r="BM40" s="29">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="41" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG41" s="26">
+        <v>18</v>
+      </c>
+      <c r="AH41" s="27">
+        <v>576</v>
+      </c>
+      <c r="AI41" s="28">
+        <v>577</v>
+      </c>
+      <c r="AJ41" s="28">
+        <v>578</v>
+      </c>
+      <c r="AK41" s="28">
+        <v>579</v>
+      </c>
+      <c r="AL41" s="28">
+        <v>580</v>
+      </c>
+      <c r="AM41" s="28">
+        <v>581</v>
+      </c>
+      <c r="AN41" s="28">
+        <v>582</v>
+      </c>
+      <c r="AO41" s="28">
+        <v>583</v>
+      </c>
+      <c r="AP41" s="28">
+        <v>584</v>
+      </c>
+      <c r="AQ41" s="28">
+        <v>585</v>
+      </c>
+      <c r="AR41" s="28">
+        <v>586</v>
+      </c>
+      <c r="AS41" s="28">
+        <v>587</v>
+      </c>
+      <c r="AT41" s="28">
+        <v>588</v>
+      </c>
+      <c r="AU41" s="28">
+        <v>589</v>
+      </c>
+      <c r="AV41" s="28">
+        <v>590</v>
+      </c>
+      <c r="AW41" s="28">
+        <v>591</v>
+      </c>
+      <c r="AX41" s="28">
+        <v>592</v>
+      </c>
+      <c r="AY41" s="28">
+        <v>593</v>
+      </c>
+      <c r="AZ41" s="28">
+        <v>594</v>
+      </c>
+      <c r="BA41" s="28">
+        <v>595</v>
+      </c>
+      <c r="BB41" s="28">
+        <v>596</v>
+      </c>
+      <c r="BC41" s="28">
+        <v>597</v>
+      </c>
+      <c r="BD41" s="28">
+        <v>598</v>
+      </c>
+      <c r="BE41" s="28">
+        <v>599</v>
+      </c>
+      <c r="BF41" s="28">
+        <v>600</v>
+      </c>
+      <c r="BG41" s="28">
+        <v>601</v>
+      </c>
+      <c r="BH41" s="28">
+        <v>602</v>
+      </c>
+      <c r="BI41" s="28">
+        <v>603</v>
+      </c>
+      <c r="BJ41" s="28">
+        <v>604</v>
+      </c>
+      <c r="BK41" s="28">
+        <v>605</v>
+      </c>
+      <c r="BL41" s="28">
+        <v>606</v>
+      </c>
+      <c r="BM41" s="29">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="42" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG42" s="26">
+        <v>19</v>
+      </c>
+      <c r="AH42" s="27">
+        <v>608</v>
+      </c>
+      <c r="AI42" s="28">
+        <v>609</v>
+      </c>
+      <c r="AJ42" s="28">
+        <v>610</v>
+      </c>
+      <c r="AK42" s="28">
+        <v>611</v>
+      </c>
+      <c r="AL42" s="28">
+        <v>612</v>
+      </c>
+      <c r="AM42" s="28">
+        <v>613</v>
+      </c>
+      <c r="AN42" s="28">
+        <v>614</v>
+      </c>
+      <c r="AO42" s="28">
+        <v>615</v>
+      </c>
+      <c r="AP42" s="28">
+        <v>616</v>
+      </c>
+      <c r="AQ42" s="28">
+        <v>617</v>
+      </c>
+      <c r="AR42" s="28">
+        <v>618</v>
+      </c>
+      <c r="AS42" s="28">
+        <v>619</v>
+      </c>
+      <c r="AT42" s="28">
+        <v>620</v>
+      </c>
+      <c r="AU42" s="28">
+        <v>621</v>
+      </c>
+      <c r="AV42" s="28">
+        <v>622</v>
+      </c>
+      <c r="AW42" s="28">
+        <v>623</v>
+      </c>
+      <c r="AX42" s="28">
+        <v>624</v>
+      </c>
+      <c r="AY42" s="28">
+        <v>625</v>
+      </c>
+      <c r="AZ42" s="28">
+        <v>626</v>
+      </c>
+      <c r="BA42" s="28">
+        <v>627</v>
+      </c>
+      <c r="BB42" s="28">
+        <v>628</v>
+      </c>
+      <c r="BC42" s="28">
+        <v>629</v>
+      </c>
+      <c r="BD42" s="28">
+        <v>630</v>
+      </c>
+      <c r="BE42" s="28">
+        <v>631</v>
+      </c>
+      <c r="BF42" s="28">
+        <v>632</v>
+      </c>
+      <c r="BG42" s="28">
+        <v>633</v>
+      </c>
+      <c r="BH42" s="28">
+        <v>634</v>
+      </c>
+      <c r="BI42" s="28">
+        <v>635</v>
+      </c>
+      <c r="BJ42" s="28">
+        <v>636</v>
+      </c>
+      <c r="BK42" s="28">
+        <v>637</v>
+      </c>
+      <c r="BL42" s="28">
+        <v>638</v>
+      </c>
+      <c r="BM42" s="29">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="43" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG43" s="26">
+        <v>20</v>
+      </c>
+      <c r="AH43" s="27">
+        <v>640</v>
+      </c>
+      <c r="AI43" s="28">
+        <v>641</v>
+      </c>
+      <c r="AJ43" s="28">
+        <v>642</v>
+      </c>
+      <c r="AK43" s="28">
+        <v>643</v>
+      </c>
+      <c r="AL43" s="28">
+        <v>644</v>
+      </c>
+      <c r="AM43" s="28">
+        <v>645</v>
+      </c>
+      <c r="AN43" s="28">
+        <v>646</v>
+      </c>
+      <c r="AO43" s="28">
+        <v>647</v>
+      </c>
+      <c r="AP43" s="28">
+        <v>648</v>
+      </c>
+      <c r="AQ43" s="28">
+        <v>649</v>
+      </c>
+      <c r="AR43" s="28">
+        <v>650</v>
+      </c>
+      <c r="AS43" s="28">
+        <v>651</v>
+      </c>
+      <c r="AT43" s="28">
+        <v>652</v>
+      </c>
+      <c r="AU43" s="28">
+        <v>653</v>
+      </c>
+      <c r="AV43" s="28">
+        <v>654</v>
+      </c>
+      <c r="AW43" s="28">
+        <v>655</v>
+      </c>
+      <c r="AX43" s="28">
+        <v>656</v>
+      </c>
+      <c r="AY43" s="28">
+        <v>657</v>
+      </c>
+      <c r="AZ43" s="28">
+        <v>658</v>
+      </c>
+      <c r="BA43" s="28">
+        <v>659</v>
+      </c>
+      <c r="BB43" s="28">
+        <v>660</v>
+      </c>
+      <c r="BC43" s="28">
+        <v>661</v>
+      </c>
+      <c r="BD43" s="28">
+        <v>662</v>
+      </c>
+      <c r="BE43" s="28">
+        <v>663</v>
+      </c>
+      <c r="BF43" s="28">
+        <v>664</v>
+      </c>
+      <c r="BG43" s="28">
+        <v>665</v>
+      </c>
+      <c r="BH43" s="28">
+        <v>666</v>
+      </c>
+      <c r="BI43" s="28">
+        <v>667</v>
+      </c>
+      <c r="BJ43" s="28">
+        <v>668</v>
+      </c>
+      <c r="BK43" s="28">
+        <v>669</v>
+      </c>
+      <c r="BL43" s="28">
+        <v>670</v>
+      </c>
+      <c r="BM43" s="29">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="44" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG44" s="26">
+        <v>21</v>
+      </c>
+      <c r="AH44" s="27">
+        <v>672</v>
+      </c>
+      <c r="AI44" s="28">
+        <v>673</v>
+      </c>
+      <c r="AJ44" s="28">
+        <v>674</v>
+      </c>
+      <c r="AK44" s="28">
+        <v>675</v>
+      </c>
+      <c r="AL44" s="28">
+        <v>676</v>
+      </c>
+      <c r="AM44" s="28">
+        <v>677</v>
+      </c>
+      <c r="AN44" s="28">
+        <v>678</v>
+      </c>
+      <c r="AO44" s="28">
+        <v>679</v>
+      </c>
+      <c r="AP44" s="28">
+        <v>680</v>
+      </c>
+      <c r="AQ44" s="28">
+        <v>681</v>
+      </c>
+      <c r="AR44" s="28">
+        <v>682</v>
+      </c>
+      <c r="AS44" s="28">
+        <v>683</v>
+      </c>
+      <c r="AT44" s="28">
+        <v>684</v>
+      </c>
+      <c r="AU44" s="28">
+        <v>685</v>
+      </c>
+      <c r="AV44" s="28">
+        <v>686</v>
+      </c>
+      <c r="AW44" s="28">
+        <v>687</v>
+      </c>
+      <c r="AX44" s="28">
+        <v>688</v>
+      </c>
+      <c r="AY44" s="28">
+        <v>689</v>
+      </c>
+      <c r="AZ44" s="28">
+        <v>690</v>
+      </c>
+      <c r="BA44" s="28">
+        <v>691</v>
+      </c>
+      <c r="BB44" s="28">
+        <v>692</v>
+      </c>
+      <c r="BC44" s="28">
+        <v>693</v>
+      </c>
+      <c r="BD44" s="28">
+        <v>694</v>
+      </c>
+      <c r="BE44" s="28">
+        <v>695</v>
+      </c>
+      <c r="BF44" s="28">
+        <v>696</v>
+      </c>
+      <c r="BG44" s="28">
+        <v>697</v>
+      </c>
+      <c r="BH44" s="28">
+        <v>698</v>
+      </c>
+      <c r="BI44" s="28">
+        <v>699</v>
+      </c>
+      <c r="BJ44" s="28">
+        <v>700</v>
+      </c>
+      <c r="BK44" s="28">
+        <v>701</v>
+      </c>
+      <c r="BL44" s="28">
+        <v>702</v>
+      </c>
+      <c r="BM44" s="29">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="45" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG45" s="26">
+        <v>22</v>
+      </c>
+      <c r="AH45" s="27">
+        <v>704</v>
+      </c>
+      <c r="AI45" s="28">
+        <v>705</v>
+      </c>
+      <c r="AJ45" s="28">
+        <v>706</v>
+      </c>
+      <c r="AK45" s="28">
+        <v>707</v>
+      </c>
+      <c r="AL45" s="28">
+        <v>708</v>
+      </c>
+      <c r="AM45" s="28">
+        <v>709</v>
+      </c>
+      <c r="AN45" s="28">
+        <v>710</v>
+      </c>
+      <c r="AO45" s="28">
+        <v>711</v>
+      </c>
+      <c r="AP45" s="28">
+        <v>712</v>
+      </c>
+      <c r="AQ45" s="28">
+        <v>713</v>
+      </c>
+      <c r="AR45" s="28">
+        <v>714</v>
+      </c>
+      <c r="AS45" s="28">
+        <v>715</v>
+      </c>
+      <c r="AT45" s="28">
+        <v>716</v>
+      </c>
+      <c r="AU45" s="28">
+        <v>717</v>
+      </c>
+      <c r="AV45" s="28">
+        <v>718</v>
+      </c>
+      <c r="AW45" s="28">
+        <v>719</v>
+      </c>
+      <c r="AX45" s="28">
+        <v>720</v>
+      </c>
+      <c r="AY45" s="28">
+        <v>721</v>
+      </c>
+      <c r="AZ45" s="28">
+        <v>722</v>
+      </c>
+      <c r="BA45" s="28">
+        <v>723</v>
+      </c>
+      <c r="BB45" s="28">
+        <v>724</v>
+      </c>
+      <c r="BC45" s="28">
+        <v>725</v>
+      </c>
+      <c r="BD45" s="28">
+        <v>726</v>
+      </c>
+      <c r="BE45" s="28">
+        <v>727</v>
+      </c>
+      <c r="BF45" s="28">
+        <v>728</v>
+      </c>
+      <c r="BG45" s="28">
+        <v>729</v>
+      </c>
+      <c r="BH45" s="28">
+        <v>730</v>
+      </c>
+      <c r="BI45" s="28">
+        <v>731</v>
+      </c>
+      <c r="BJ45" s="28">
+        <v>732</v>
+      </c>
+      <c r="BK45" s="28">
+        <v>733</v>
+      </c>
+      <c r="BL45" s="28">
+        <v>734</v>
+      </c>
+      <c r="BM45" s="29">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="46" spans="33:65" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG46" s="26">
+        <v>23</v>
+      </c>
+      <c r="AH46" s="37">
+        <v>736</v>
+      </c>
+      <c r="AI46" s="35">
+        <v>737</v>
+      </c>
+      <c r="AJ46" s="35">
+        <v>738</v>
+      </c>
+      <c r="AK46" s="35">
+        <v>739</v>
+      </c>
+      <c r="AL46" s="35">
+        <v>740</v>
+      </c>
+      <c r="AM46" s="35">
+        <v>741</v>
+      </c>
+      <c r="AN46" s="35">
+        <v>742</v>
+      </c>
+      <c r="AO46" s="35">
+        <v>743</v>
+      </c>
+      <c r="AP46" s="35">
+        <v>744</v>
+      </c>
+      <c r="AQ46" s="35">
+        <v>745</v>
+      </c>
+      <c r="AR46" s="35">
+        <v>746</v>
+      </c>
+      <c r="AS46" s="35">
+        <v>747</v>
+      </c>
+      <c r="AT46" s="35">
+        <v>748</v>
+      </c>
+      <c r="AU46" s="35">
+        <v>749</v>
+      </c>
+      <c r="AV46" s="35">
+        <v>750</v>
+      </c>
+      <c r="AW46" s="35">
+        <v>751</v>
+      </c>
+      <c r="AX46" s="35">
+        <v>752</v>
+      </c>
+      <c r="AY46" s="35">
+        <v>753</v>
+      </c>
+      <c r="AZ46" s="35">
+        <v>754</v>
+      </c>
+      <c r="BA46" s="35">
+        <v>755</v>
+      </c>
+      <c r="BB46" s="35">
+        <v>756</v>
+      </c>
+      <c r="BC46" s="35">
+        <v>757</v>
+      </c>
+      <c r="BD46" s="35">
+        <v>758</v>
+      </c>
+      <c r="BE46" s="35">
+        <v>759</v>
+      </c>
+      <c r="BF46" s="35">
+        <v>760</v>
+      </c>
+      <c r="BG46" s="35">
+        <v>761</v>
+      </c>
+      <c r="BH46" s="35">
+        <v>762</v>
+      </c>
+      <c r="BI46" s="35">
+        <v>763</v>
+      </c>
+      <c r="BJ46" s="35">
+        <v>764</v>
+      </c>
+      <c r="BK46" s="35">
+        <v>765</v>
+      </c>
+      <c r="BL46" s="35">
+        <v>766</v>
+      </c>
+      <c r="BM46" s="36">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="47" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH47" s="38"/>
+      <c r="AI47" s="38"/>
+      <c r="AJ47" s="38"/>
+      <c r="AK47" s="38"/>
+      <c r="AL47" s="38"/>
+      <c r="AM47" s="38"/>
+      <c r="AN47" s="38"/>
+      <c r="AO47" s="38"/>
+      <c r="AP47" s="38"/>
+      <c r="AQ47" s="38"/>
+      <c r="AR47" s="38"/>
+      <c r="AS47" s="38"/>
+      <c r="AT47" s="38"/>
+      <c r="AU47" s="38"/>
+      <c r="AV47" s="38"/>
+      <c r="AW47" s="38"/>
+      <c r="AX47" s="38"/>
+      <c r="AY47" s="38"/>
+      <c r="AZ47" s="38"/>
+      <c r="BA47" s="38"/>
+      <c r="BB47" s="38"/>
+      <c r="BC47" s="38"/>
+      <c r="BD47" s="38"/>
+      <c r="BE47" s="38"/>
+      <c r="BF47" s="38"/>
+      <c r="BG47" s="38"/>
+      <c r="BH47" s="38"/>
+      <c r="BI47" s="38"/>
+      <c r="BJ47" s="38"/>
+      <c r="BK47" s="38"/>
+      <c r="BL47" s="38"/>
+      <c r="BM47" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AR21:BC21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B249DA5-B757-4EDE-957B-043D98EC57E6}">
   <dimension ref="A1:BM47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
@@ -728,20 +3483,20 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="19" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AR19" s="11" t="s">
+      <c r="AR19" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AS19" s="11"/>
-      <c r="AT19" s="11"/>
-      <c r="AU19" s="11"/>
-      <c r="AV19" s="11"/>
-      <c r="AW19" s="11"/>
-      <c r="AX19" s="11"/>
-      <c r="AY19" s="11"/>
-      <c r="AZ19" s="11"/>
-      <c r="BA19" s="11"/>
-      <c r="BB19" s="11"/>
-      <c r="BC19" s="11"/>
+      <c r="AS19" s="22"/>
+      <c r="AT19" s="22"/>
+      <c r="AU19" s="22"/>
+      <c r="AV19" s="22"/>
+      <c r="AW19" s="22"/>
+      <c r="AX19" s="22"/>
+      <c r="AY19" s="22"/>
+      <c r="AZ19" s="22"/>
+      <c r="BA19" s="22"/>
+      <c r="BB19" s="22"/>
+      <c r="BC19" s="22"/>
     </row>
     <row r="22" spans="33:65" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AH22" s="4">
@@ -845,17 +3600,17 @@
       <c r="AG23" s="4">
         <v>0</v>
       </c>
-      <c r="AH23" s="21"/>
-      <c r="AI23" s="15"/>
-      <c r="AJ23" s="15"/>
+      <c r="AH23" s="20"/>
+      <c r="AI23" s="14"/>
+      <c r="AJ23" s="14"/>
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
-      <c r="AP23" s="15"/>
-      <c r="AQ23" s="15"/>
-      <c r="AR23" s="15"/>
+      <c r="AP23" s="14"/>
+      <c r="AQ23" s="14"/>
+      <c r="AR23" s="14"/>
       <c r="AS23" s="2"/>
       <c r="AT23" s="2"/>
       <c r="AU23" s="2"/>
@@ -882,7 +3637,7 @@
       <c r="AG24" s="4">
         <v>1</v>
       </c>
-      <c r="AH24" s="20"/>
+      <c r="AH24" s="19"/>
       <c r="AI24" s="6"/>
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
@@ -890,7 +3645,7 @@
       <c r="AM24" s="6"/>
       <c r="AN24" s="6"/>
       <c r="AO24" s="6"/>
-      <c r="AP24" s="22"/>
+      <c r="AP24" s="21"/>
       <c r="AQ24" s="6"/>
       <c r="AR24" s="6"/>
       <c r="AS24" s="6"/>
@@ -919,7 +3674,7 @@
       <c r="AG25" s="4">
         <v>2</v>
       </c>
-      <c r="AH25" s="17"/>
+      <c r="AH25" s="16"/>
       <c r="AI25" s="6"/>
       <c r="AJ25" s="6"/>
       <c r="AK25" s="6"/>
@@ -927,7 +3682,7 @@
       <c r="AM25" s="6"/>
       <c r="AN25" s="6"/>
       <c r="AO25" s="6"/>
-      <c r="AP25" s="19"/>
+      <c r="AP25" s="18"/>
       <c r="AQ25" s="6"/>
       <c r="AR25" s="6"/>
       <c r="AS25" s="6"/>
@@ -1775,7 +4530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B2FA38-8D4B-4969-9313-513A9A5DD9FE}">
   <dimension ref="A1:BM47"/>
   <sheetViews>
@@ -1891,20 +4646,20 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="19" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AR19" s="11" t="s">
+      <c r="AR19" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AS19" s="11"/>
-      <c r="AT19" s="11"/>
-      <c r="AU19" s="11"/>
-      <c r="AV19" s="11"/>
-      <c r="AW19" s="11"/>
-      <c r="AX19" s="11"/>
-      <c r="AY19" s="11"/>
-      <c r="AZ19" s="11"/>
-      <c r="BA19" s="11"/>
-      <c r="BB19" s="11"/>
-      <c r="BC19" s="11"/>
+      <c r="AS19" s="22"/>
+      <c r="AT19" s="22"/>
+      <c r="AU19" s="22"/>
+      <c r="AV19" s="22"/>
+      <c r="AW19" s="22"/>
+      <c r="AX19" s="22"/>
+      <c r="AY19" s="22"/>
+      <c r="AZ19" s="22"/>
+      <c r="BA19" s="22"/>
+      <c r="BB19" s="22"/>
+      <c r="BC19" s="22"/>
     </row>
     <row r="22" spans="33:65" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AH22" s="4">
@@ -2008,17 +4763,17 @@
       <c r="AG23" s="4">
         <v>0</v>
       </c>
-      <c r="AH23" s="18"/>
-      <c r="AI23" s="15"/>
-      <c r="AJ23" s="15"/>
+      <c r="AH23" s="17"/>
+      <c r="AI23" s="14"/>
+      <c r="AJ23" s="14"/>
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
-      <c r="AP23" s="14"/>
-      <c r="AQ23" s="15"/>
-      <c r="AR23" s="15"/>
+      <c r="AP23" s="13"/>
+      <c r="AQ23" s="14"/>
+      <c r="AR23" s="14"/>
       <c r="AS23" s="2"/>
       <c r="AT23" s="2"/>
       <c r="AU23" s="2"/>
@@ -2045,7 +4800,7 @@
       <c r="AG24" s="4">
         <v>1</v>
       </c>
-      <c r="AH24" s="17"/>
+      <c r="AH24" s="16"/>
       <c r="AI24" s="6"/>
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
@@ -2053,7 +4808,7 @@
       <c r="AM24" s="6"/>
       <c r="AN24" s="6"/>
       <c r="AO24" s="6"/>
-      <c r="AP24" s="19"/>
+      <c r="AP24" s="18"/>
       <c r="AQ24" s="6"/>
       <c r="AR24" s="6"/>
       <c r="AS24" s="6"/>
@@ -2938,7 +5693,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0657AC-A7BC-4E1A-851F-870AC4BE46C5}">
   <dimension ref="A1:BM47"/>
   <sheetViews>
@@ -3054,20 +5809,20 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="19" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AR19" s="11" t="s">
+      <c r="AR19" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AS19" s="11"/>
-      <c r="AT19" s="11"/>
-      <c r="AU19" s="11"/>
-      <c r="AV19" s="11"/>
-      <c r="AW19" s="11"/>
-      <c r="AX19" s="11"/>
-      <c r="AY19" s="11"/>
-      <c r="AZ19" s="11"/>
-      <c r="BA19" s="11"/>
-      <c r="BB19" s="11"/>
-      <c r="BC19" s="11"/>
+      <c r="AS19" s="22"/>
+      <c r="AT19" s="22"/>
+      <c r="AU19" s="22"/>
+      <c r="AV19" s="22"/>
+      <c r="AW19" s="22"/>
+      <c r="AX19" s="22"/>
+      <c r="AY19" s="22"/>
+      <c r="AZ19" s="22"/>
+      <c r="BA19" s="22"/>
+      <c r="BB19" s="22"/>
+      <c r="BC19" s="22"/>
     </row>
     <row r="22" spans="33:65" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AH22" s="4">
@@ -3171,17 +5926,17 @@
       <c r="AG23" s="4">
         <v>0</v>
       </c>
-      <c r="AH23" s="16"/>
-      <c r="AI23" s="14"/>
-      <c r="AJ23" s="15"/>
+      <c r="AH23" s="15"/>
+      <c r="AI23" s="13"/>
+      <c r="AJ23" s="14"/>
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
-      <c r="AP23" s="13"/>
-      <c r="AQ23" s="12"/>
-      <c r="AR23" s="15"/>
+      <c r="AP23" s="12"/>
+      <c r="AQ23" s="11"/>
+      <c r="AR23" s="14"/>
       <c r="AS23" s="2"/>
       <c r="AT23" s="2"/>
       <c r="AU23" s="2"/>
@@ -4101,7 +6856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33AF7E0-E4FE-4EFE-9910-4AF5B6B5E759}">
   <dimension ref="A1:BM47"/>
   <sheetViews>
@@ -4217,20 +6972,20 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="19" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AR19" s="11" t="s">
+      <c r="AR19" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AS19" s="11"/>
-      <c r="AT19" s="11"/>
-      <c r="AU19" s="11"/>
-      <c r="AV19" s="11"/>
-      <c r="AW19" s="11"/>
-      <c r="AX19" s="11"/>
-      <c r="AY19" s="11"/>
-      <c r="AZ19" s="11"/>
-      <c r="BA19" s="11"/>
-      <c r="BB19" s="11"/>
-      <c r="BC19" s="11"/>
+      <c r="AS19" s="22"/>
+      <c r="AT19" s="22"/>
+      <c r="AU19" s="22"/>
+      <c r="AV19" s="22"/>
+      <c r="AW19" s="22"/>
+      <c r="AX19" s="22"/>
+      <c r="AY19" s="22"/>
+      <c r="AZ19" s="22"/>
+      <c r="BA19" s="22"/>
+      <c r="BB19" s="22"/>
+      <c r="BC19" s="22"/>
     </row>
     <row r="22" spans="33:65" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AH22" s="4">
@@ -4335,16 +7090,16 @@
         <v>0</v>
       </c>
       <c r="AH23" s="1"/>
-      <c r="AI23" s="13"/>
-      <c r="AJ23" s="14"/>
+      <c r="AI23" s="12"/>
+      <c r="AJ23" s="13"/>
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
       <c r="AP23" s="2"/>
-      <c r="AQ23" s="13"/>
-      <c r="AR23" s="14"/>
+      <c r="AQ23" s="12"/>
+      <c r="AR23" s="13"/>
       <c r="AS23" s="2"/>
       <c r="AT23" s="2"/>
       <c r="AU23" s="2"/>
@@ -5264,7 +8019,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD2516C-D626-4902-BF5B-E33EDD53A0BC}">
   <dimension ref="A1:BM47"/>
   <sheetViews>
@@ -5380,20 +8135,20 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="19" spans="33:65" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AR19" s="11" t="s">
+      <c r="AR19" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AS19" s="11"/>
-      <c r="AT19" s="11"/>
-      <c r="AU19" s="11"/>
-      <c r="AV19" s="11"/>
-      <c r="AW19" s="11"/>
-      <c r="AX19" s="11"/>
-      <c r="AY19" s="11"/>
-      <c r="AZ19" s="11"/>
-      <c r="BA19" s="11"/>
-      <c r="BB19" s="11"/>
-      <c r="BC19" s="11"/>
+      <c r="AS19" s="22"/>
+      <c r="AT19" s="22"/>
+      <c r="AU19" s="22"/>
+      <c r="AV19" s="22"/>
+      <c r="AW19" s="22"/>
+      <c r="AX19" s="22"/>
+      <c r="AY19" s="22"/>
+      <c r="AZ19" s="22"/>
+      <c r="BA19" s="22"/>
+      <c r="BB19" s="22"/>
+      <c r="BC19" s="22"/>
     </row>
     <row r="22" spans="33:65" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AH22" s="4">
@@ -5498,16 +8253,16 @@
         <v>0</v>
       </c>
       <c r="AH23" s="1"/>
-      <c r="AI23" s="12"/>
-      <c r="AJ23" s="13"/>
+      <c r="AI23" s="11"/>
+      <c r="AJ23" s="12"/>
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
       <c r="AP23" s="2"/>
-      <c r="AQ23" s="14"/>
-      <c r="AR23" s="13"/>
+      <c r="AQ23" s="13"/>
+      <c r="AR23" s="12"/>
       <c r="AS23" s="2"/>
       <c r="AT23" s="2"/>
       <c r="AU23" s="2"/>

</xml_diff>